<commit_message>
UI updates, Lecturer Selection modals
</commit_message>
<xml_diff>
--- a/public/Timetable_Input_Template.xlsx
+++ b/public/Timetable_Input_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\Timetable-Scheduler-Fullstack\Frontend\PAU-Timetable_Scheduler\Input System Details\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\PAU-Timetable_Scheduler\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85745CD3-5E43-41EB-8177-BA62783345BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7CAFE7-8BE5-43DC-99F2-6EFF2276B7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lecturers" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Room Name</t>
   </si>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="105" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1197,7 +1197,11 @@
       <c r="A134"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F2" xr:uid="{9F4F4CBA-0FC0-4749-A916-A40DACB90D67}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{EC9FC771-7554-440F-A483-EEFE119E6A07}">
+      <formula1>"Full-Time, Adjunct"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1207,7 +1211,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1235,15 +1239,18 @@
       <c r="E1" s="18"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SST, TYD"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D3:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Classroom, Phy Lab, Chem Lab, Hall, Workshop, Comp Lab, Fluid Mech Lab, Mechanics Lab, Materials Lab, Thermo Lab, Studio"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{FC95F02B-0D39-48CD-A4FB-CA8979CED481}">
+      <formula1>"Classroom, Physics Lab, Chemistry Lab, Hall, Workshop, Computer Lab, Fluid Mech Lab, Mechanics Lab, Materials Lab, Thermo Lab, Studio"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1252,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1265,9 +1272,10 @@
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -1283,13 +1291,22 @@
       <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1048576" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{ACF7EC3E-DDC4-4AB9-8D46-626130CC9A9B}">
+      <formula1>"100, 200, 300, 400, 500"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{DFFBF27D-0F0B-4BB2-8A60-D2B2A90033D0}">
+      <formula1>"SST, TYD"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1299,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L272"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1534,7 +1551,11 @@
       <c r="F272" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{1321D10E-A6DA-4FDA-8FDA-F689E6D8C1FF}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{9E117DCC-4746-41A6-AA44-8F272011D14D}">
+      <formula1>"Classroom, Physics Lab, Chemistry Lab, Hall, Workshop, Computer Lab, Fluid Mech Lab, Mechanics Lab, Materials Lab, Thermo Lab, Studio"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>